<commit_message>
Se realizaron pruebas de conexión con odbc, ole, a la base de datos , ajustes a la aplicación
* problemas de conexión de Oracle por tema de 64 bits
Se investigo la manera de consumir fuente de datos a 32 bits
Se realizo la configuración de envió de correo con la cuenta de hotmail.
Se dieron reversa a las conexión realizadas
</commit_message>
<xml_diff>
--- a/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/reportes/web_reports/BOSCH/Transmision_EDOCs_18975_may-01-2024may-31-2024.xlsx
+++ b/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/reportes/web_reports/BOSCH/Transmision_EDOCs_18975_may-01-2024may-31-2024.xlsx
@@ -6,8 +6,8 @@
     <x:workbookView activeTab="1"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Exportación" sheetId="1" r:id="Rce3e701d6855414a"/>
-    <x:sheet name="Importación" sheetId="2" r:id="Re073cc5186274123"/>
+    <x:sheet name="Exportación" sheetId="1" r:id="Rc3791ba567e6491f"/>
+    <x:sheet name="Importación" sheetId="2" r:id="R27e53dc01b2e42eb"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -123,16 +123,16 @@
     <x:t>09/05/2024</x:t>
   </x:si>
   <x:si>
+    <x:t>4001128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22/05/2024</x:t>
+  </x:si>
+  <x:si>
     <x:t>4001099</x:t>
   </x:si>
   <x:si>
     <x:t>20/05/2024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4001128</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22/05/2024</x:t>
   </x:si>
   <x:si>
     <x:t>4001100</x:t>
@@ -1153,7 +1153,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E18" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F18" s="2" t="s">
         <x:v>37</x:v>
@@ -1176,7 +1176,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E19" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F19" s="2" t="s">
         <x:v>39</x:v>
@@ -1271,7 +1271,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F23" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G23" s="2">
         <x:v>5</x:v>
@@ -2008,7 +2008,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="F22" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G22" s="2">
         <x:v>2</x:v>
@@ -2031,7 +2031,7 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="F23" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G23" s="2">
         <x:v>7</x:v>
@@ -2192,7 +2192,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="F30" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G30" s="2">
         <x:v>2</x:v>
@@ -2284,7 +2284,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F34" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G34" s="2">
         <x:v>7</x:v>
@@ -2330,7 +2330,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F36" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G36" s="2">
         <x:v>8</x:v>
@@ -2353,7 +2353,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F37" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G37" s="2">
         <x:v>4</x:v>
@@ -2422,7 +2422,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F40" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G40" s="2">
         <x:v>1</x:v>

</xml_diff>

<commit_message>
agregar excepciones en la aplicación en conexiones
agregar configuración app.config para conexión de BD
 agregar configuración app.config y secrets  , y pruebas con la NVA BD ORFEODES
</commit_message>
<xml_diff>
--- a/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/reportes/web_reports/BOSCH/Transmision_EDOCs_18975_may-01-2024may-31-2024.xlsx
+++ b/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/reportes/web_reports/BOSCH/Transmision_EDOCs_18975_may-01-2024may-31-2024.xlsx
@@ -6,8 +6,8 @@
     <x:workbookView activeTab="1"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Exportación" sheetId="1" r:id="Rc3791ba567e6491f"/>
-    <x:sheet name="Importación" sheetId="2" r:id="R27e53dc01b2e42eb"/>
+    <x:sheet name="Exportación" sheetId="1" r:id="R80c61d7a03374a78"/>
+    <x:sheet name="Importación" sheetId="2" r:id="Rf77dc70d1b9f4748"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -54,6 +54,12 @@
     <x:t>03/05/2024</x:t>
   </x:si>
   <x:si>
+    <x:t>4001081</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08/05/2024</x:t>
+  </x:si>
+  <x:si>
     <x:t>4000834</x:t>
   </x:si>
   <x:si>
@@ -63,12 +69,6 @@
     <x:t>07/05/2024</x:t>
   </x:si>
   <x:si>
-    <x:t>4001081</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08/05/2024</x:t>
-  </x:si>
-  <x:si>
     <x:t>4000895</x:t>
   </x:si>
   <x:si>
@@ -93,13 +93,13 @@
     <x:t>15/05/2024</x:t>
   </x:si>
   <x:si>
+    <x:t>4001070</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16/05/2024</x:t>
+  </x:si>
+  <x:si>
     <x:t>4001130</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16/05/2024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4001070</x:t>
   </x:si>
   <x:si>
     <x:t>4001071</x:t>
@@ -808,10 +808,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="F3" s="2" t="s">
-        <x:v>15</x:v>
       </x:c>
       <x:c r="G3" s="2">
         <x:v>15</x:v>
@@ -825,13 +825,13 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D4" s="2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D4" s="2">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E4" s="2" t="s">
-        <x:v>11</x:v>
       </x:c>
       <x:c r="F4" s="2" t="s">
         <x:v>17</x:v>
@@ -854,10 +854,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F5" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G5" s="2">
         <x:v>6</x:v>
@@ -900,7 +900,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E7" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F7" s="2" t="s">
         <x:v>12</x:v>
@@ -926,7 +926,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F8" s="2" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G8" s="2">
         <x:v>5</x:v>
@@ -949,7 +949,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F9" s="2" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G9" s="2">
         <x:v>5</x:v>
@@ -969,7 +969,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E10" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F10" s="2" t="s">
         <x:v>25</x:v>
@@ -992,7 +992,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E11" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F11" s="2" t="s">
         <x:v>27</x:v>
@@ -1015,7 +1015,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E12" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F12" s="2" t="s">
         <x:v>27</x:v>
@@ -1038,7 +1038,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E13" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F13" s="2" t="s">
         <x:v>25</x:v>
@@ -1107,10 +1107,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="F16" s="2" t="s">
-        <x:v>17</x:v>
       </x:c>
       <x:c r="G16" s="2">
         <x:v>7</x:v>
@@ -1176,7 +1176,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E19" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F19" s="2" t="s">
         <x:v>39</x:v>
@@ -1199,7 +1199,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E20" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F20" s="2" t="s">
         <x:v>41</x:v>
@@ -1360,7 +1360,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E27" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F27" s="2" t="s">
         <x:v>53</x:v>
@@ -1383,7 +1383,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E28" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F28" s="2" t="s">
         <x:v>53</x:v>
@@ -1406,7 +1406,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E29" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F29" s="2" t="s">
         <x:v>53</x:v>
@@ -1429,7 +1429,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E30" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F30" s="2" t="s">
         <x:v>57</x:v>
@@ -1475,7 +1475,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E32" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F32" s="2" t="s">
         <x:v>51</x:v>
@@ -1594,7 +1594,7 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="F4" s="2" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G4" s="2">
         <x:v>54</x:v>
@@ -1617,7 +1617,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="F5" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G5" s="2">
         <x:v>2</x:v>
@@ -1640,7 +1640,7 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="F6" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G6" s="2">
         <x:v>2</x:v>
@@ -1732,7 +1732,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="F10" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G10" s="2">
         <x:v>2</x:v>
@@ -1778,7 +1778,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F12" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G12" s="2">
         <x:v>10</x:v>
@@ -1801,7 +1801,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="F13" s="2" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G13" s="2">
         <x:v>9</x:v>

</xml_diff>